<commit_message>
Highly improved collisions (collision with the "ceiling" still remaining)
</commit_message>
<xml_diff>
--- a/Tasks delivered.xlsx
+++ b/Tasks delivered.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\usuario\Documents\GitHub\The-Cliffborn-Islands\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{99EDC6CC-A6D3-4565-B772-C75B6941A0C6}" xr6:coauthVersionLast="37" xr6:coauthVersionMax="37" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1C4FA606-18AA-4475-81E0-A652F6B89447}" xr6:coauthVersionLast="37" xr6:coauthVersionMax="37" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="21570" windowHeight="8430" activeTab="1" xr2:uid="{8AEDAC0E-C01A-427C-877A-819CB7AFB0CE}"/>
   </bookViews>
@@ -16,7 +16,7 @@
     <sheet name="Hoja1" sheetId="1" r:id="rId1"/>
     <sheet name="Hoja2" sheetId="2" r:id="rId2"/>
   </sheets>
-  <calcPr calcId="179021"/>
+  <calcPr calcId="162913"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -26,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="57" uniqueCount="41">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="60" uniqueCount="44">
   <si>
     <t>These are the taks delivered to create The Cliffborn Islands</t>
   </si>
@@ -149,6 +149,15 @@
   </si>
   <si>
     <t>Delivery date</t>
+  </si>
+  <si>
+    <t>Created the sprites of godmode and implemented it</t>
+  </si>
+  <si>
+    <t>45 minutes</t>
+  </si>
+  <si>
+    <t>1h 15 minutes</t>
   </si>
 </sst>
 </file>
@@ -362,7 +371,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="26">
+  <cellXfs count="27">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
@@ -395,6 +404,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -1118,7 +1128,7 @@
   <dimension ref="B1:I22"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="J8" sqref="J8"/>
+      <selection activeCell="L13" sqref="L13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1323,6 +1333,23 @@
         <v>43381</v>
       </c>
     </row>
+    <row r="18" spans="2:9" x14ac:dyDescent="0.25">
+      <c r="C18" s="22" t="s">
+        <v>41</v>
+      </c>
+      <c r="D18" s="23"/>
+      <c r="E18" s="23"/>
+      <c r="F18" s="24"/>
+      <c r="G18" s="26" t="s">
+        <v>42</v>
+      </c>
+      <c r="H18" s="1" t="s">
+        <v>43</v>
+      </c>
+      <c r="I18" s="18">
+        <v>43385</v>
+      </c>
+    </row>
     <row r="19" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B19" s="2"/>
       <c r="C19" s="1"/>

</xml_diff>